<commit_message>
update zeitkonto installed docker
</commit_message>
<xml_diff>
--- a/Zeitkonto_DKE.xlsx
+++ b/Zeitkonto_DKE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EEBE31-82F3-420F-B1A3-728D568EE28B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A6ADC-F17D-4DCE-9F4A-48856FD9366B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgaben" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>Thomas</t>
+  </si>
+  <si>
+    <t>Fr</t>
+  </si>
+  <si>
+    <t>Di</t>
   </si>
 </sst>
 </file>
@@ -478,7 +484,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -860,6 +866,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="98">
@@ -1422,7 +1431,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -1733,7 +1742,7 @@
   </sheetPr>
   <dimension ref="A1:G632"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1827,7 +1836,7 @@
       <c r="D7" s="33"/>
       <c r="E7" s="34">
         <f ca="1">INDIRECT("'"&amp;A7&amp;"'!G4")</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="28" customFormat="1" ht="15.75">
@@ -1852,7 +1861,7 @@
       <c r="D9" s="39"/>
       <c r="E9" s="40">
         <f ca="1">SUM(E5:E8)</f>
-        <v>23.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="44" customFormat="1" ht="13.5" thickTop="1">
@@ -9907,8 +9916,8 @@
   </sheetPr>
   <dimension ref="A1:G916"/>
   <sheetViews>
-    <sheetView topLeftCell="A315" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F355"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
@@ -23962,8 +23971,8 @@
   </sheetPr>
   <dimension ref="A1:G916"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
@@ -23973,7 +23982,7 @@
     <col min="3" max="3" width="6.28515625" style="90" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" style="91" customWidth="1"/>
     <col min="5" max="5" width="21.140625" style="92" customWidth="1"/>
-    <col min="6" max="6" width="24" style="93" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" style="93" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" style="93" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.85546875" style="94"/>
   </cols>
@@ -24023,7 +24032,7 @@
       </c>
       <c r="G4" s="67">
         <f>SUM(G7:G996)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="74" customFormat="1" ht="15.75">
@@ -24137,51 +24146,65 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="81" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B10" s="103"/>
-      <c r="C10" s="104"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="106" t="str">
+      <c r="A10" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="86">
+        <v>44120</v>
+      </c>
+      <c r="C10" s="87">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D10" s="87">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E10" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="85" t="str">
         <f>IF(ISBLANK(E10),"",VLOOKUP(E10,Aufgaben!A:B,2,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G10" s="31" t="str">
+        <v>Entwicklungsumgebung vorbereiten</v>
+      </c>
+      <c r="G10" s="31">
+        <f>IF(B10&lt;&gt;"",IF(D10&lt;C10,1-C10+D10,D10-C10)*24,"")</f>
+        <v>2.0000000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75">
+      <c r="A11" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="86">
+        <v>44117</v>
+      </c>
+      <c r="C11" s="87">
+        <v>0.625</v>
+      </c>
+      <c r="D11" s="87">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E11" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="85" t="str">
+        <f>IF(ISBLANK(E11),"",VLOOKUP(E11,Aufgaben!A:B,2,FALSE))</f>
+        <v>Teammeeting</v>
+      </c>
+      <c r="G11" s="31">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="81" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B11" s="103"/>
-      <c r="C11" s="104"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="106" t="str">
-        <f>IF(ISBLANK(E11),"",VLOOKUP(E11,Aufgaben!A:B,2,FALSE))</f>
-        <v/>
-      </c>
-      <c r="G11" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>2.0000000000000009</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75">
       <c r="A12" s="81" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B12" s="103"/>
-      <c r="C12" s="104"/>
-      <c r="D12" s="104"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="106" t="str">
+        <f>IF(B12&lt;&gt;"",TEXT(B12,"TTT"),"")</f>
+        <v/>
+      </c>
+      <c r="B12" s="86"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="85" t="str">
         <f>IF(ISBLANK(E12),"",VLOOKUP(E12,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24195,11 +24218,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B13" s="103"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="106" t="str">
+      <c r="B13" s="86"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="85" t="str">
         <f>IF(ISBLANK(E13),"",VLOOKUP(E13,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24213,11 +24236,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B14" s="103"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="106" t="str">
+      <c r="B14" s="86"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="85" t="str">
         <f>IF(ISBLANK(E14),"",VLOOKUP(E14,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24231,11 +24254,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B15" s="103"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="106" t="str">
+      <c r="B15" s="86"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="85" t="str">
         <f>IF(ISBLANK(E15),"",VLOOKUP(E15,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24249,11 +24272,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B16" s="103"/>
-      <c r="C16" s="104"/>
-      <c r="D16" s="104"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="106" t="str">
+      <c r="B16" s="86"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="128"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="85" t="str">
         <f>IF(ISBLANK(E16),"",VLOOKUP(E16,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24267,11 +24290,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B17" s="103"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="106" t="str">
+      <c r="B17" s="86"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="128"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="85" t="str">
         <f>IF(ISBLANK(E17),"",VLOOKUP(E17,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24285,11 +24308,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B18" s="103"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="106" t="str">
+      <c r="B18" s="86"/>
+      <c r="C18" s="128"/>
+      <c r="D18" s="128"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="85" t="str">
         <f>IF(ISBLANK(E18),"",VLOOKUP(E18,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24303,11 +24326,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B19" s="103"/>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="105"/>
-      <c r="F19" s="106" t="str">
+      <c r="B19" s="86"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="85" t="str">
         <f>IF(ISBLANK(E19),"",VLOOKUP(E19,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24321,11 +24344,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B20" s="103"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="106" t="str">
+      <c r="B20" s="86"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="85" t="str">
         <f>IF(ISBLANK(E20),"",VLOOKUP(E20,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24339,11 +24362,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B21" s="103"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="106" t="str">
+      <c r="B21" s="86"/>
+      <c r="C21" s="128"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="85" t="str">
         <f>IF(ISBLANK(E21),"",VLOOKUP(E21,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24357,11 +24380,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B22" s="103"/>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="106" t="str">
+      <c r="B22" s="86"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="85" t="str">
         <f>IF(ISBLANK(E22),"",VLOOKUP(E22,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24375,11 +24398,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B23" s="103"/>
-      <c r="C23" s="104"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="106" t="str">
+      <c r="B23" s="86"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="85" t="str">
         <f>IF(ISBLANK(E23),"",VLOOKUP(E23,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24393,11 +24416,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B24" s="103"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="106" t="str">
+      <c r="B24" s="86"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="85" t="str">
         <f>IF(ISBLANK(E24),"",VLOOKUP(E24,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24411,11 +24434,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B25" s="103"/>
-      <c r="C25" s="104"/>
-      <c r="D25" s="104"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="106" t="str">
+      <c r="B25" s="86"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="85" t="str">
         <f>IF(ISBLANK(E25),"",VLOOKUP(E25,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24429,11 +24452,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B26" s="103"/>
-      <c r="C26" s="104"/>
-      <c r="D26" s="104"/>
-      <c r="E26" s="105"/>
-      <c r="F26" s="106" t="str">
+      <c r="B26" s="86"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="85" t="str">
         <f>IF(ISBLANK(E26),"",VLOOKUP(E26,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24447,11 +24470,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B27" s="103"/>
-      <c r="C27" s="104"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="106" t="str">
+      <c r="B27" s="86"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="85" t="str">
         <f>IF(ISBLANK(E27),"",VLOOKUP(E27,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24465,11 +24488,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="104"/>
-      <c r="D28" s="104"/>
-      <c r="E28" s="105"/>
-      <c r="F28" s="106" t="str">
+      <c r="B28" s="86"/>
+      <c r="C28" s="128"/>
+      <c r="D28" s="128"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="85" t="str">
         <f>IF(ISBLANK(E28),"",VLOOKUP(E28,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24483,11 +24506,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B29" s="103"/>
-      <c r="C29" s="104"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="105"/>
-      <c r="F29" s="106" t="str">
+      <c r="B29" s="86"/>
+      <c r="C29" s="128"/>
+      <c r="D29" s="128"/>
+      <c r="E29" s="84"/>
+      <c r="F29" s="85" t="str">
         <f>IF(ISBLANK(E29),"",VLOOKUP(E29,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24501,11 +24524,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B30" s="103"/>
-      <c r="C30" s="104"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="105"/>
-      <c r="F30" s="106" t="str">
+      <c r="B30" s="86"/>
+      <c r="C30" s="128"/>
+      <c r="D30" s="128"/>
+      <c r="E30" s="84"/>
+      <c r="F30" s="85" t="str">
         <f>IF(ISBLANK(E30),"",VLOOKUP(E30,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24519,11 +24542,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B31" s="103"/>
-      <c r="C31" s="104"/>
-      <c r="D31" s="104"/>
-      <c r="E31" s="105"/>
-      <c r="F31" s="106" t="str">
+      <c r="B31" s="86"/>
+      <c r="C31" s="128"/>
+      <c r="D31" s="128"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="85" t="str">
         <f>IF(ISBLANK(E31),"",VLOOKUP(E31,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24537,11 +24560,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B32" s="103"/>
-      <c r="C32" s="104"/>
-      <c r="D32" s="104"/>
-      <c r="E32" s="105"/>
-      <c r="F32" s="106" t="str">
+      <c r="B32" s="86"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="85" t="str">
         <f>IF(ISBLANK(E32),"",VLOOKUP(E32,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24555,11 +24578,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B33" s="103"/>
-      <c r="C33" s="104"/>
-      <c r="D33" s="104"/>
-      <c r="E33" s="105"/>
-      <c r="F33" s="106" t="str">
+      <c r="B33" s="86"/>
+      <c r="C33" s="128"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="85" t="str">
         <f>IF(ISBLANK(E33),"",VLOOKUP(E33,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24573,11 +24596,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B34" s="103"/>
-      <c r="C34" s="104"/>
-      <c r="D34" s="104"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="106" t="str">
+      <c r="B34" s="86"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="85" t="str">
         <f>IF(ISBLANK(E34),"",VLOOKUP(E34,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>
@@ -24591,11 +24614,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B35" s="103"/>
-      <c r="C35" s="104"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="105"/>
-      <c r="F35" s="106" t="str">
+      <c r="B35" s="86"/>
+      <c r="C35" s="128"/>
+      <c r="D35" s="128"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="85" t="str">
         <f>IF(ISBLANK(E35),"",VLOOKUP(E35,Aufgaben!A:B,2,FALSE))</f>
         <v/>
       </c>

</xml_diff>